<commit_message>
update hour sprint 1
</commit_message>
<xml_diff>
--- a/5.Print-Backlog/Sprint-1.xlsx
+++ b/5.Print-Backlog/Sprint-1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\caps1\5.Print-Backlog\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Actual" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="47">
   <si>
     <t>No</t>
   </si>
@@ -174,6 +169,9 @@
   </si>
   <si>
     <t>Code front-end for playtime</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -375,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -466,6 +464,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,6 +490,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -789,12 +811,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1838620688"/>
-        <c:axId val="1838606544"/>
+        <c:axId val="201655424"/>
+        <c:axId val="201656960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="1838620688"/>
+        <c:axId val="201655424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,14 +827,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1838606544"/>
+        <c:crossAx val="201656960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="1838606544"/>
+        <c:axId val="201656960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,7 +845,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1838620688"/>
+        <c:crossAx val="201655424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -921,7 +944,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -956,7 +979,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1165,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE38"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,38 +1308,76 @@
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="42">
         <v>1</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="43">
         <v>1</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
+      <c r="G2" s="44">
+        <v>0</v>
+      </c>
+      <c r="H2" s="44">
+        <v>0</v>
+      </c>
+      <c r="I2" s="44">
+        <v>0</v>
+      </c>
+      <c r="J2" s="44">
+        <v>0</v>
+      </c>
+      <c r="K2" s="44">
+        <v>0</v>
+      </c>
+      <c r="L2" s="44">
+        <v>0</v>
+      </c>
+      <c r="M2" s="44">
+        <v>0</v>
+      </c>
+      <c r="N2" s="44">
+        <v>0</v>
+      </c>
+      <c r="O2" s="44">
+        <v>0</v>
+      </c>
+      <c r="P2" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="44">
+        <v>0</v>
+      </c>
+      <c r="R2" s="44">
+        <v>0</v>
+      </c>
+      <c r="S2" s="44">
+        <v>0</v>
+      </c>
+      <c r="T2" s="44">
+        <v>0</v>
+      </c>
+      <c r="U2" s="44">
+        <v>0</v>
+      </c>
+      <c r="V2" s="44">
+        <v>0</v>
+      </c>
+      <c r="W2" s="44">
+        <v>0</v>
+      </c>
+      <c r="X2" s="44">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="44">
+        <v>0</v>
+      </c>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
@@ -1328,36 +1389,76 @@
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="14" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="32">
         <v>1</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
+      <c r="F3" s="43">
+        <v>1</v>
+      </c>
+      <c r="G3" s="44">
+        <v>0</v>
+      </c>
+      <c r="H3" s="44">
+        <v>0</v>
+      </c>
+      <c r="I3" s="44">
+        <v>0</v>
+      </c>
+      <c r="J3" s="44">
+        <v>0</v>
+      </c>
+      <c r="K3" s="44">
+        <v>0</v>
+      </c>
+      <c r="L3" s="44">
+        <v>0</v>
+      </c>
+      <c r="M3" s="44">
+        <v>0</v>
+      </c>
+      <c r="N3" s="44">
+        <v>0</v>
+      </c>
+      <c r="O3" s="44">
+        <v>0</v>
+      </c>
+      <c r="P3" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="44">
+        <v>0</v>
+      </c>
+      <c r="R3" s="44">
+        <v>0</v>
+      </c>
+      <c r="S3" s="44">
+        <v>0</v>
+      </c>
+      <c r="T3" s="44">
+        <v>0</v>
+      </c>
+      <c r="U3" s="44">
+        <v>0</v>
+      </c>
+      <c r="V3" s="44">
+        <v>0</v>
+      </c>
+      <c r="W3" s="44">
+        <v>0</v>
+      </c>
+      <c r="X3" s="44">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="44">
+        <v>0</v>
+      </c>
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
       <c r="AB3" s="8"/>
@@ -1369,7 +1470,7 @@
       <c r="A4" s="28">
         <v>3</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -1378,29 +1479,69 @@
       <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="32">
         <v>2</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
+      <c r="F4" s="43">
+        <v>2</v>
+      </c>
+      <c r="G4" s="43">
+        <v>0</v>
+      </c>
+      <c r="H4" s="43">
+        <v>0</v>
+      </c>
+      <c r="I4" s="43">
+        <v>0</v>
+      </c>
+      <c r="J4" s="43">
+        <v>0</v>
+      </c>
+      <c r="K4" s="43">
+        <v>0</v>
+      </c>
+      <c r="L4" s="43">
+        <v>0</v>
+      </c>
+      <c r="M4" s="43">
+        <v>0</v>
+      </c>
+      <c r="N4" s="43">
+        <v>0</v>
+      </c>
+      <c r="O4" s="43">
+        <v>0</v>
+      </c>
+      <c r="P4" s="43">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="43">
+        <v>0</v>
+      </c>
+      <c r="R4" s="43">
+        <v>0</v>
+      </c>
+      <c r="S4" s="43">
+        <v>0</v>
+      </c>
+      <c r="T4" s="43">
+        <v>0</v>
+      </c>
+      <c r="U4" s="43">
+        <v>0</v>
+      </c>
+      <c r="V4" s="43">
+        <v>0</v>
+      </c>
+      <c r="W4" s="43">
+        <v>0</v>
+      </c>
+      <c r="X4" s="43">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="43">
+        <v>0</v>
+      </c>
       <c r="Z4" s="8"/>
       <c r="AA4" s="8"/>
       <c r="AB4" s="8"/>
@@ -1412,36 +1553,76 @@
       <c r="A5" s="28">
         <v>4</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="32">
         <v>2</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="24"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
+      <c r="F5" s="43">
+        <v>0</v>
+      </c>
+      <c r="G5" s="43">
+        <v>2</v>
+      </c>
+      <c r="H5" s="45">
+        <v>0</v>
+      </c>
+      <c r="I5" s="45">
+        <v>0</v>
+      </c>
+      <c r="J5" s="45">
+        <v>0</v>
+      </c>
+      <c r="K5" s="45">
+        <v>0</v>
+      </c>
+      <c r="L5" s="45">
+        <v>0</v>
+      </c>
+      <c r="M5" s="45">
+        <v>0</v>
+      </c>
+      <c r="N5" s="45">
+        <v>0</v>
+      </c>
+      <c r="O5" s="45">
+        <v>0</v>
+      </c>
+      <c r="P5" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="45">
+        <v>0</v>
+      </c>
+      <c r="R5" s="45">
+        <v>0</v>
+      </c>
+      <c r="S5" s="45">
+        <v>0</v>
+      </c>
+      <c r="T5" s="45">
+        <v>0</v>
+      </c>
+      <c r="U5" s="45">
+        <v>0</v>
+      </c>
+      <c r="V5" s="45">
+        <v>0</v>
+      </c>
+      <c r="W5" s="45">
+        <v>0</v>
+      </c>
+      <c r="X5" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="45">
+        <v>0</v>
+      </c>
       <c r="Z5" s="8"/>
       <c r="AA5" s="8"/>
       <c r="AB5" s="8"/>
@@ -1453,36 +1634,76 @@
       <c r="A6" s="28">
         <v>5</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="14" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="32">
         <v>1</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="24"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
+      <c r="F6" s="43">
+        <v>0</v>
+      </c>
+      <c r="G6" s="43">
+        <v>1</v>
+      </c>
+      <c r="H6" s="45">
+        <v>0</v>
+      </c>
+      <c r="I6" s="45">
+        <v>0</v>
+      </c>
+      <c r="J6" s="45">
+        <v>0</v>
+      </c>
+      <c r="K6" s="45">
+        <v>0</v>
+      </c>
+      <c r="L6" s="45">
+        <v>0</v>
+      </c>
+      <c r="M6" s="45">
+        <v>0</v>
+      </c>
+      <c r="N6" s="45">
+        <v>0</v>
+      </c>
+      <c r="O6" s="45">
+        <v>0</v>
+      </c>
+      <c r="P6" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="45">
+        <v>0</v>
+      </c>
+      <c r="R6" s="45">
+        <v>0</v>
+      </c>
+      <c r="S6" s="45">
+        <v>0</v>
+      </c>
+      <c r="T6" s="45">
+        <v>0</v>
+      </c>
+      <c r="U6" s="45">
+        <v>0</v>
+      </c>
+      <c r="V6" s="45">
+        <v>0</v>
+      </c>
+      <c r="W6" s="45">
+        <v>0</v>
+      </c>
+      <c r="X6" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="45">
+        <v>0</v>
+      </c>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
       <c r="AB6" s="8"/>
@@ -1494,36 +1715,76 @@
       <c r="A7" s="28">
         <v>6</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="14" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="32">
         <v>6</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="24"/>
-      <c r="T7" s="24"/>
-      <c r="U7" s="24"/>
-      <c r="V7" s="24"/>
-      <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
+      <c r="F7" s="43">
+        <v>0</v>
+      </c>
+      <c r="G7" s="43">
+        <v>1</v>
+      </c>
+      <c r="H7" s="45">
+        <v>4</v>
+      </c>
+      <c r="I7" s="46">
+        <v>1</v>
+      </c>
+      <c r="J7" s="46">
+        <v>0</v>
+      </c>
+      <c r="K7" s="46">
+        <v>0</v>
+      </c>
+      <c r="L7" s="46">
+        <v>0</v>
+      </c>
+      <c r="M7" s="46">
+        <v>0</v>
+      </c>
+      <c r="N7" s="46">
+        <v>0</v>
+      </c>
+      <c r="O7" s="46">
+        <v>0</v>
+      </c>
+      <c r="P7" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="46">
+        <v>0</v>
+      </c>
+      <c r="R7" s="46">
+        <v>0</v>
+      </c>
+      <c r="S7" s="46">
+        <v>0</v>
+      </c>
+      <c r="T7" s="46">
+        <v>0</v>
+      </c>
+      <c r="U7" s="46">
+        <v>0</v>
+      </c>
+      <c r="V7" s="46">
+        <v>0</v>
+      </c>
+      <c r="W7" s="46">
+        <v>0</v>
+      </c>
+      <c r="X7" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="46">
+        <v>0</v>
+      </c>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8"/>
       <c r="AB7" s="8"/>
@@ -1535,7 +1796,7 @@
       <c r="A8" s="28">
         <v>7</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1544,29 +1805,69 @@
       <c r="D8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="32">
         <v>1</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
-      <c r="S8" s="24"/>
-      <c r="T8" s="24"/>
-      <c r="U8" s="24"/>
-      <c r="V8" s="24"/>
-      <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
+      <c r="F8" s="43">
+        <v>0</v>
+      </c>
+      <c r="G8" s="43">
+        <v>0</v>
+      </c>
+      <c r="H8" s="43">
+        <v>0</v>
+      </c>
+      <c r="I8" s="46">
+        <v>1</v>
+      </c>
+      <c r="J8" s="46">
+        <v>0</v>
+      </c>
+      <c r="K8" s="46">
+        <v>0</v>
+      </c>
+      <c r="L8" s="46">
+        <v>0</v>
+      </c>
+      <c r="M8" s="46">
+        <v>0</v>
+      </c>
+      <c r="N8" s="46">
+        <v>0</v>
+      </c>
+      <c r="O8" s="46">
+        <v>0</v>
+      </c>
+      <c r="P8" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="46">
+        <v>0</v>
+      </c>
+      <c r="R8" s="46">
+        <v>0</v>
+      </c>
+      <c r="S8" s="46">
+        <v>0</v>
+      </c>
+      <c r="T8" s="46">
+        <v>0</v>
+      </c>
+      <c r="U8" s="46">
+        <v>0</v>
+      </c>
+      <c r="V8" s="46">
+        <v>0</v>
+      </c>
+      <c r="W8" s="46">
+        <v>0</v>
+      </c>
+      <c r="X8" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="46">
+        <v>0</v>
+      </c>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
@@ -1578,36 +1879,76 @@
       <c r="A9" s="28">
         <v>8</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="32">
         <v>2</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
+      <c r="F9" s="43">
+        <v>0</v>
+      </c>
+      <c r="G9" s="43">
+        <v>0</v>
+      </c>
+      <c r="H9" s="43">
+        <v>0</v>
+      </c>
+      <c r="I9" s="46">
+        <v>2</v>
+      </c>
+      <c r="J9" s="45">
+        <v>0</v>
+      </c>
+      <c r="K9" s="45">
+        <v>0</v>
+      </c>
+      <c r="L9" s="45">
+        <v>0</v>
+      </c>
+      <c r="M9" s="45">
+        <v>0</v>
+      </c>
+      <c r="N9" s="45">
+        <v>0</v>
+      </c>
+      <c r="O9" s="45">
+        <v>0</v>
+      </c>
+      <c r="P9" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="45">
+        <v>0</v>
+      </c>
+      <c r="R9" s="45">
+        <v>0</v>
+      </c>
+      <c r="S9" s="45">
+        <v>0</v>
+      </c>
+      <c r="T9" s="45">
+        <v>0</v>
+      </c>
+      <c r="U9" s="45">
+        <v>0</v>
+      </c>
+      <c r="V9" s="45">
+        <v>0</v>
+      </c>
+      <c r="W9" s="45">
+        <v>0</v>
+      </c>
+      <c r="X9" s="45">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="45">
+        <v>0</v>
+      </c>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
       <c r="AB9" s="8"/>
@@ -1619,36 +1960,76 @@
       <c r="A10" s="28">
         <v>9</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="14" t="s">
         <v>40</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="32">
         <v>1</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
-      <c r="U10" s="24"/>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="24"/>
-      <c r="Y10" s="24"/>
+      <c r="F10" s="43">
+        <v>0</v>
+      </c>
+      <c r="G10" s="43">
+        <v>0</v>
+      </c>
+      <c r="H10" s="43">
+        <v>0</v>
+      </c>
+      <c r="I10" s="46">
+        <v>0</v>
+      </c>
+      <c r="J10" s="47">
+        <v>1</v>
+      </c>
+      <c r="K10" s="46">
+        <v>0</v>
+      </c>
+      <c r="L10" s="46">
+        <v>0</v>
+      </c>
+      <c r="M10" s="46">
+        <v>0</v>
+      </c>
+      <c r="N10" s="46">
+        <v>0</v>
+      </c>
+      <c r="O10" s="46">
+        <v>0</v>
+      </c>
+      <c r="P10" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="46">
+        <v>0</v>
+      </c>
+      <c r="R10" s="46">
+        <v>0</v>
+      </c>
+      <c r="S10" s="46">
+        <v>0</v>
+      </c>
+      <c r="T10" s="46">
+        <v>0</v>
+      </c>
+      <c r="U10" s="46">
+        <v>0</v>
+      </c>
+      <c r="V10" s="46">
+        <v>0</v>
+      </c>
+      <c r="W10" s="46">
+        <v>0</v>
+      </c>
+      <c r="X10" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="46">
+        <v>0</v>
+      </c>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8"/>
       <c r="AB10" s="8"/>
@@ -1660,36 +2041,76 @@
       <c r="A11" s="28">
         <v>10</v>
       </c>
-      <c r="B11" s="35"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="32">
         <v>2</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24"/>
+      <c r="F11" s="43">
+        <v>0</v>
+      </c>
+      <c r="G11" s="43">
+        <v>0</v>
+      </c>
+      <c r="H11" s="43">
+        <v>0</v>
+      </c>
+      <c r="I11" s="46">
+        <v>0</v>
+      </c>
+      <c r="J11" s="45">
+        <v>2</v>
+      </c>
+      <c r="K11" s="46">
+        <v>0</v>
+      </c>
+      <c r="L11" s="46">
+        <v>0</v>
+      </c>
+      <c r="M11" s="46">
+        <v>0</v>
+      </c>
+      <c r="N11" s="46">
+        <v>0</v>
+      </c>
+      <c r="O11" s="46">
+        <v>0</v>
+      </c>
+      <c r="P11" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="46">
+        <v>0</v>
+      </c>
+      <c r="R11" s="46">
+        <v>0</v>
+      </c>
+      <c r="S11" s="46">
+        <v>0</v>
+      </c>
+      <c r="T11" s="46">
+        <v>0</v>
+      </c>
+      <c r="U11" s="46">
+        <v>0</v>
+      </c>
+      <c r="V11" s="46">
+        <v>0</v>
+      </c>
+      <c r="W11" s="46">
+        <v>0</v>
+      </c>
+      <c r="X11" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="46">
+        <v>0</v>
+      </c>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
       <c r="AB11" s="8"/>
@@ -1701,7 +2122,7 @@
       <c r="A12" s="28">
         <v>11</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="37" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -1710,29 +2131,69 @@
       <c r="D12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="32">
         <v>2</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
+      <c r="F12" s="43">
+        <v>0</v>
+      </c>
+      <c r="G12" s="43">
+        <v>0</v>
+      </c>
+      <c r="H12" s="43">
+        <v>0</v>
+      </c>
+      <c r="I12" s="46">
+        <v>0</v>
+      </c>
+      <c r="J12" s="47">
+        <v>1</v>
+      </c>
+      <c r="K12" s="46">
+        <v>1</v>
+      </c>
+      <c r="L12" s="46">
+        <v>0</v>
+      </c>
+      <c r="M12" s="46">
+        <v>0</v>
+      </c>
+      <c r="N12" s="46">
+        <v>0</v>
+      </c>
+      <c r="O12" s="46">
+        <v>0</v>
+      </c>
+      <c r="P12" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="46">
+        <v>0</v>
+      </c>
+      <c r="R12" s="46">
+        <v>0</v>
+      </c>
+      <c r="S12" s="46">
+        <v>0</v>
+      </c>
+      <c r="T12" s="46">
+        <v>0</v>
+      </c>
+      <c r="U12" s="46">
+        <v>0</v>
+      </c>
+      <c r="V12" s="46">
+        <v>0</v>
+      </c>
+      <c r="W12" s="46">
+        <v>0</v>
+      </c>
+      <c r="X12" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="46">
+        <v>0</v>
+      </c>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8"/>
       <c r="AB12" s="8"/>
@@ -1744,36 +2205,76 @@
       <c r="A13" s="28">
         <v>12</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="14" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="32">
         <v>8</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="24"/>
-      <c r="V13" s="24"/>
-      <c r="W13" s="24"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="24"/>
+      <c r="F13" s="46">
+        <v>0</v>
+      </c>
+      <c r="G13" s="46">
+        <v>0</v>
+      </c>
+      <c r="H13" s="46">
+        <v>0</v>
+      </c>
+      <c r="I13" s="46">
+        <v>0</v>
+      </c>
+      <c r="J13" s="46">
+        <v>0</v>
+      </c>
+      <c r="K13" s="45">
+        <v>3</v>
+      </c>
+      <c r="L13" s="46">
+        <v>4</v>
+      </c>
+      <c r="M13" s="46">
+        <v>1</v>
+      </c>
+      <c r="N13" s="46">
+        <v>0</v>
+      </c>
+      <c r="O13" s="46">
+        <v>0</v>
+      </c>
+      <c r="P13" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="46">
+        <v>0</v>
+      </c>
+      <c r="R13" s="46">
+        <v>0</v>
+      </c>
+      <c r="S13" s="46">
+        <v>0</v>
+      </c>
+      <c r="T13" s="46">
+        <v>0</v>
+      </c>
+      <c r="U13" s="46">
+        <v>0</v>
+      </c>
+      <c r="V13" s="46">
+        <v>0</v>
+      </c>
+      <c r="W13" s="46">
+        <v>0</v>
+      </c>
+      <c r="X13" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="46">
+        <v>0</v>
+      </c>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8"/>
       <c r="AB13" s="8"/>
@@ -1785,36 +2286,76 @@
       <c r="A14" s="28">
         <v>13</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="20" t="s">
         <v>42</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="32">
         <v>6</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="24"/>
-      <c r="V14" s="24"/>
-      <c r="W14" s="24"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
+      <c r="F14" s="46">
+        <v>0</v>
+      </c>
+      <c r="G14" s="45">
+        <v>0</v>
+      </c>
+      <c r="H14" s="45">
+        <v>0</v>
+      </c>
+      <c r="I14" s="46">
+        <v>0</v>
+      </c>
+      <c r="J14" s="46">
+        <v>0</v>
+      </c>
+      <c r="K14" s="46">
+        <v>0</v>
+      </c>
+      <c r="L14" s="46">
+        <v>0</v>
+      </c>
+      <c r="M14" s="46">
+        <v>3</v>
+      </c>
+      <c r="N14" s="46">
+        <v>3</v>
+      </c>
+      <c r="O14" s="46">
+        <v>0</v>
+      </c>
+      <c r="P14" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="46">
+        <v>0</v>
+      </c>
+      <c r="R14" s="46">
+        <v>0</v>
+      </c>
+      <c r="S14" s="46">
+        <v>0</v>
+      </c>
+      <c r="T14" s="46">
+        <v>0</v>
+      </c>
+      <c r="U14" s="46">
+        <v>0</v>
+      </c>
+      <c r="V14" s="46">
+        <v>0</v>
+      </c>
+      <c r="W14" s="46">
+        <v>0</v>
+      </c>
+      <c r="X14" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="46">
+        <v>0</v>
+      </c>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
       <c r="AB14" s="8"/>
@@ -1826,7 +2367,7 @@
       <c r="A15" s="28">
         <v>14</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="34" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="21" t="s">
@@ -1835,29 +2376,69 @@
       <c r="D15" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="32">
         <v>3</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
-      <c r="W15" s="24"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
+      <c r="F15" s="46">
+        <v>0</v>
+      </c>
+      <c r="G15" s="45">
+        <v>0</v>
+      </c>
+      <c r="H15" s="45">
+        <v>0</v>
+      </c>
+      <c r="I15" s="46">
+        <v>0</v>
+      </c>
+      <c r="J15" s="46">
+        <v>0</v>
+      </c>
+      <c r="K15" s="46">
+        <v>0</v>
+      </c>
+      <c r="L15" s="46">
+        <v>0</v>
+      </c>
+      <c r="M15" s="46">
+        <v>0</v>
+      </c>
+      <c r="N15" s="46">
+        <v>1</v>
+      </c>
+      <c r="O15" s="46">
+        <v>2</v>
+      </c>
+      <c r="P15" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="46">
+        <v>0</v>
+      </c>
+      <c r="R15" s="46">
+        <v>0</v>
+      </c>
+      <c r="S15" s="46">
+        <v>0</v>
+      </c>
+      <c r="T15" s="46">
+        <v>0</v>
+      </c>
+      <c r="U15" s="46">
+        <v>0</v>
+      </c>
+      <c r="V15" s="46">
+        <v>0</v>
+      </c>
+      <c r="W15" s="46">
+        <v>0</v>
+      </c>
+      <c r="X15" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="46">
+        <v>0</v>
+      </c>
       <c r="Z15" s="8"/>
       <c r="AA15" s="8"/>
       <c r="AB15" s="8"/>
@@ -1869,36 +2450,76 @@
       <c r="A16" s="28">
         <v>15</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="14" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="32">
         <v>4</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="24"/>
-      <c r="V16" s="24"/>
-      <c r="W16" s="24"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
+      <c r="F16" s="46">
+        <v>0</v>
+      </c>
+      <c r="G16" s="45">
+        <v>0</v>
+      </c>
+      <c r="H16" s="45">
+        <v>0</v>
+      </c>
+      <c r="I16" s="46">
+        <v>0</v>
+      </c>
+      <c r="J16" s="46">
+        <v>0</v>
+      </c>
+      <c r="K16" s="46">
+        <v>0</v>
+      </c>
+      <c r="L16" s="46">
+        <v>0</v>
+      </c>
+      <c r="M16" s="46">
+        <v>0</v>
+      </c>
+      <c r="N16" s="46">
+        <v>0</v>
+      </c>
+      <c r="O16" s="46">
+        <v>2</v>
+      </c>
+      <c r="P16" s="46">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="46">
+        <v>0</v>
+      </c>
+      <c r="R16" s="46">
+        <v>0</v>
+      </c>
+      <c r="S16" s="46">
+        <v>0</v>
+      </c>
+      <c r="T16" s="46">
+        <v>0</v>
+      </c>
+      <c r="U16" s="46">
+        <v>0</v>
+      </c>
+      <c r="V16" s="46">
+        <v>0</v>
+      </c>
+      <c r="W16" s="46">
+        <v>0</v>
+      </c>
+      <c r="X16" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="46">
+        <v>0</v>
+      </c>
       <c r="Z16" s="8"/>
       <c r="AA16" s="8"/>
       <c r="AB16" s="8"/>
@@ -1910,36 +2531,76 @@
       <c r="A17" s="28">
         <v>16</v>
       </c>
-      <c r="B17" s="32"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="32">
         <v>3</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="24"/>
-      <c r="Y17" s="24"/>
+      <c r="F17" s="46">
+        <v>0</v>
+      </c>
+      <c r="G17" s="45">
+        <v>0</v>
+      </c>
+      <c r="H17" s="45">
+        <v>0</v>
+      </c>
+      <c r="I17" s="46">
+        <v>0</v>
+      </c>
+      <c r="J17" s="46">
+        <v>0</v>
+      </c>
+      <c r="K17" s="46">
+        <v>0</v>
+      </c>
+      <c r="L17" s="46">
+        <v>0</v>
+      </c>
+      <c r="M17" s="46">
+        <v>0</v>
+      </c>
+      <c r="N17" s="46">
+        <v>0</v>
+      </c>
+      <c r="O17" s="46">
+        <v>0</v>
+      </c>
+      <c r="P17" s="46">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="46">
+        <v>1</v>
+      </c>
+      <c r="R17" s="46">
+        <v>0</v>
+      </c>
+      <c r="S17" s="46">
+        <v>0</v>
+      </c>
+      <c r="T17" s="46">
+        <v>0</v>
+      </c>
+      <c r="U17" s="46">
+        <v>0</v>
+      </c>
+      <c r="V17" s="46">
+        <v>0</v>
+      </c>
+      <c r="W17" s="46">
+        <v>0</v>
+      </c>
+      <c r="X17" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="46">
+        <v>0</v>
+      </c>
       <c r="Z17" s="8"/>
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
@@ -1951,36 +2612,76 @@
       <c r="A18" s="28">
         <v>17</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="32">
         <v>15</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="24"/>
+      <c r="F18" s="46">
+        <v>0</v>
+      </c>
+      <c r="G18" s="45">
+        <v>0</v>
+      </c>
+      <c r="H18" s="45">
+        <v>0</v>
+      </c>
+      <c r="I18" s="46">
+        <v>0</v>
+      </c>
+      <c r="J18" s="46">
+        <v>0</v>
+      </c>
+      <c r="K18" s="46">
+        <v>0</v>
+      </c>
+      <c r="L18" s="46">
+        <v>0</v>
+      </c>
+      <c r="M18" s="46">
+        <v>0</v>
+      </c>
+      <c r="N18" s="46">
+        <v>0</v>
+      </c>
+      <c r="O18" s="46">
+        <v>0</v>
+      </c>
+      <c r="P18" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="46">
+        <v>3</v>
+      </c>
+      <c r="R18" s="46">
+        <v>4</v>
+      </c>
+      <c r="S18" s="46">
+        <v>4</v>
+      </c>
+      <c r="T18" s="46">
+        <v>4</v>
+      </c>
+      <c r="U18" s="46">
+        <v>4</v>
+      </c>
+      <c r="V18" s="46">
+        <v>0</v>
+      </c>
+      <c r="W18" s="46">
+        <v>0</v>
+      </c>
+      <c r="X18" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="46">
+        <v>0</v>
+      </c>
       <c r="Z18" s="8"/>
       <c r="AA18" s="8"/>
       <c r="AB18" s="8"/>
@@ -1992,7 +2693,7 @@
       <c r="A19" s="28">
         <v>18</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -2001,29 +2702,69 @@
       <c r="D19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="32">
         <v>1</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="24"/>
-      <c r="V19" s="24"/>
-      <c r="W19" s="24"/>
-      <c r="X19" s="24"/>
-      <c r="Y19" s="24"/>
+      <c r="F19" s="46">
+        <v>0</v>
+      </c>
+      <c r="G19" s="45">
+        <v>0</v>
+      </c>
+      <c r="H19" s="45">
+        <v>0</v>
+      </c>
+      <c r="I19" s="46">
+        <v>0</v>
+      </c>
+      <c r="J19" s="46">
+        <v>0</v>
+      </c>
+      <c r="K19" s="46">
+        <v>0</v>
+      </c>
+      <c r="L19" s="46">
+        <v>0</v>
+      </c>
+      <c r="M19" s="46">
+        <v>0</v>
+      </c>
+      <c r="N19" s="46">
+        <v>0</v>
+      </c>
+      <c r="O19" s="46">
+        <v>0</v>
+      </c>
+      <c r="P19" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="46">
+        <v>0</v>
+      </c>
+      <c r="R19" s="46">
+        <v>0</v>
+      </c>
+      <c r="S19" s="46">
+        <v>0</v>
+      </c>
+      <c r="T19" s="46">
+        <v>0</v>
+      </c>
+      <c r="U19" s="46">
+        <v>0</v>
+      </c>
+      <c r="V19" s="46">
+        <v>1</v>
+      </c>
+      <c r="W19" s="46">
+        <v>0</v>
+      </c>
+      <c r="X19" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="46">
+        <v>0</v>
+      </c>
       <c r="Z19" s="8"/>
       <c r="AA19" s="8"/>
       <c r="AB19" s="8"/>
@@ -2035,36 +2776,76 @@
       <c r="A20" s="28">
         <v>19</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="14" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="32">
         <v>2</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
-      <c r="N20" s="24"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
+      <c r="F20" s="46">
+        <v>0</v>
+      </c>
+      <c r="G20" s="45">
+        <v>0</v>
+      </c>
+      <c r="H20" s="45">
+        <v>0</v>
+      </c>
+      <c r="I20" s="46">
+        <v>0</v>
+      </c>
+      <c r="J20" s="46">
+        <v>0</v>
+      </c>
+      <c r="K20" s="46">
+        <v>0</v>
+      </c>
+      <c r="L20" s="46">
+        <v>0</v>
+      </c>
+      <c r="M20" s="46">
+        <v>0</v>
+      </c>
+      <c r="N20" s="46">
+        <v>0</v>
+      </c>
+      <c r="O20" s="46">
+        <v>0</v>
+      </c>
+      <c r="P20" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="46">
+        <v>0</v>
+      </c>
+      <c r="R20" s="46">
+        <v>0</v>
+      </c>
+      <c r="S20" s="46">
+        <v>0</v>
+      </c>
+      <c r="T20" s="46">
+        <v>0</v>
+      </c>
+      <c r="U20" s="46">
+        <v>0</v>
+      </c>
+      <c r="V20" s="46">
+        <v>2</v>
+      </c>
+      <c r="W20" s="46">
+        <v>0</v>
+      </c>
+      <c r="X20" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="46">
+        <v>0</v>
+      </c>
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
@@ -2076,36 +2857,76 @@
       <c r="A21" s="28">
         <v>20</v>
       </c>
-      <c r="B21" s="34"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="32">
         <v>1</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="24"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="24"/>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="24"/>
-      <c r="V21" s="24"/>
-      <c r="W21" s="24"/>
-      <c r="X21" s="24"/>
-      <c r="Y21" s="24"/>
+      <c r="F21" s="46">
+        <v>0</v>
+      </c>
+      <c r="G21" s="45">
+        <v>0</v>
+      </c>
+      <c r="H21" s="45">
+        <v>0</v>
+      </c>
+      <c r="I21" s="46">
+        <v>0</v>
+      </c>
+      <c r="J21" s="46">
+        <v>0</v>
+      </c>
+      <c r="K21" s="46">
+        <v>0</v>
+      </c>
+      <c r="L21" s="46">
+        <v>0</v>
+      </c>
+      <c r="M21" s="46">
+        <v>0</v>
+      </c>
+      <c r="N21" s="46">
+        <v>0</v>
+      </c>
+      <c r="O21" s="46">
+        <v>0</v>
+      </c>
+      <c r="P21" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="46">
+        <v>0</v>
+      </c>
+      <c r="R21" s="46">
+        <v>0</v>
+      </c>
+      <c r="S21" s="46">
+        <v>0</v>
+      </c>
+      <c r="T21" s="46">
+        <v>0</v>
+      </c>
+      <c r="U21" s="46">
+        <v>0</v>
+      </c>
+      <c r="V21" s="46">
+        <v>1</v>
+      </c>
+      <c r="W21" s="46">
+        <v>0</v>
+      </c>
+      <c r="X21" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="46">
+        <v>0</v>
+      </c>
       <c r="Z21" s="8"/>
       <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
@@ -2117,36 +2938,76 @@
       <c r="A22" s="28">
         <v>21</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="32">
         <v>1</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
-      <c r="T22" s="24"/>
-      <c r="U22" s="24"/>
-      <c r="V22" s="24"/>
-      <c r="W22" s="24"/>
-      <c r="X22" s="24"/>
-      <c r="Y22" s="24"/>
+      <c r="F22" s="46">
+        <v>0</v>
+      </c>
+      <c r="G22" s="45">
+        <v>0</v>
+      </c>
+      <c r="H22" s="45">
+        <v>0</v>
+      </c>
+      <c r="I22" s="46">
+        <v>0</v>
+      </c>
+      <c r="J22" s="46">
+        <v>0</v>
+      </c>
+      <c r="K22" s="46">
+        <v>0</v>
+      </c>
+      <c r="L22" s="46">
+        <v>0</v>
+      </c>
+      <c r="M22" s="46">
+        <v>0</v>
+      </c>
+      <c r="N22" s="46">
+        <v>0</v>
+      </c>
+      <c r="O22" s="46">
+        <v>0</v>
+      </c>
+      <c r="P22" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="46">
+        <v>0</v>
+      </c>
+      <c r="R22" s="46">
+        <v>0</v>
+      </c>
+      <c r="S22" s="46">
+        <v>0</v>
+      </c>
+      <c r="T22" s="46">
+        <v>0</v>
+      </c>
+      <c r="U22" s="46">
+        <v>0</v>
+      </c>
+      <c r="V22" s="46">
+        <v>0</v>
+      </c>
+      <c r="W22" s="46">
+        <v>1</v>
+      </c>
+      <c r="X22" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="46">
+        <v>0</v>
+      </c>
       <c r="Z22" s="8"/>
       <c r="AA22" s="8"/>
       <c r="AB22" s="8"/>
@@ -2158,36 +3019,76 @@
       <c r="A23" s="28">
         <v>22</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="32">
         <v>2</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
-      <c r="T23" s="24"/>
-      <c r="U23" s="24"/>
-      <c r="V23" s="24"/>
-      <c r="W23" s="24"/>
-      <c r="X23" s="24"/>
-      <c r="Y23" s="24"/>
+      <c r="F23" s="46">
+        <v>0</v>
+      </c>
+      <c r="G23" s="45">
+        <v>0</v>
+      </c>
+      <c r="H23" s="45">
+        <v>0</v>
+      </c>
+      <c r="I23" s="46">
+        <v>0</v>
+      </c>
+      <c r="J23" s="46">
+        <v>0</v>
+      </c>
+      <c r="K23" s="46">
+        <v>0</v>
+      </c>
+      <c r="L23" s="46">
+        <v>0</v>
+      </c>
+      <c r="M23" s="46">
+        <v>0</v>
+      </c>
+      <c r="N23" s="46">
+        <v>0</v>
+      </c>
+      <c r="O23" s="46">
+        <v>0</v>
+      </c>
+      <c r="P23" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="46">
+        <v>0</v>
+      </c>
+      <c r="R23" s="46">
+        <v>0</v>
+      </c>
+      <c r="S23" s="46">
+        <v>0</v>
+      </c>
+      <c r="T23" s="46">
+        <v>0</v>
+      </c>
+      <c r="U23" s="46">
+        <v>0</v>
+      </c>
+      <c r="V23" s="46">
+        <v>0</v>
+      </c>
+      <c r="W23" s="46">
+        <v>2</v>
+      </c>
+      <c r="X23" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="46">
+        <v>0</v>
+      </c>
       <c r="Z23" s="8"/>
       <c r="AA23" s="8"/>
       <c r="AB23" s="8"/>
@@ -2199,36 +3100,76 @@
       <c r="A24" s="28">
         <v>23</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="32">
         <v>1</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="24"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="24"/>
-      <c r="U24" s="24"/>
-      <c r="V24" s="24"/>
-      <c r="W24" s="24"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="24"/>
+      <c r="F24" s="46">
+        <v>0</v>
+      </c>
+      <c r="G24" s="45">
+        <v>0</v>
+      </c>
+      <c r="H24" s="45">
+        <v>0</v>
+      </c>
+      <c r="I24" s="46">
+        <v>0</v>
+      </c>
+      <c r="J24" s="46">
+        <v>0</v>
+      </c>
+      <c r="K24" s="46">
+        <v>0</v>
+      </c>
+      <c r="L24" s="46">
+        <v>0</v>
+      </c>
+      <c r="M24" s="46">
+        <v>0</v>
+      </c>
+      <c r="N24" s="46">
+        <v>0</v>
+      </c>
+      <c r="O24" s="46">
+        <v>0</v>
+      </c>
+      <c r="P24" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="46">
+        <v>0</v>
+      </c>
+      <c r="R24" s="46">
+        <v>0</v>
+      </c>
+      <c r="S24" s="46">
+        <v>0</v>
+      </c>
+      <c r="T24" s="46">
+        <v>0</v>
+      </c>
+      <c r="U24" s="46">
+        <v>0</v>
+      </c>
+      <c r="V24" s="46">
+        <v>0</v>
+      </c>
+      <c r="W24" s="46">
+        <v>1</v>
+      </c>
+      <c r="X24" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="46">
+        <v>0</v>
+      </c>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8"/>
       <c r="AB24" s="8"/>
@@ -2240,36 +3181,76 @@
       <c r="A25" s="28">
         <v>24</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="32">
         <v>1</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="24"/>
-      <c r="V25" s="24"/>
-      <c r="W25" s="24"/>
-      <c r="X25" s="24"/>
-      <c r="Y25" s="24"/>
+      <c r="F25" s="46">
+        <v>0</v>
+      </c>
+      <c r="G25" s="45">
+        <v>0</v>
+      </c>
+      <c r="H25" s="45">
+        <v>0</v>
+      </c>
+      <c r="I25" s="46">
+        <v>0</v>
+      </c>
+      <c r="J25" s="46">
+        <v>0</v>
+      </c>
+      <c r="K25" s="46">
+        <v>0</v>
+      </c>
+      <c r="L25" s="46">
+        <v>0</v>
+      </c>
+      <c r="M25" s="46">
+        <v>0</v>
+      </c>
+      <c r="N25" s="46">
+        <v>0</v>
+      </c>
+      <c r="O25" s="46">
+        <v>0</v>
+      </c>
+      <c r="P25" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="46">
+        <v>0</v>
+      </c>
+      <c r="R25" s="46">
+        <v>0</v>
+      </c>
+      <c r="S25" s="46">
+        <v>0</v>
+      </c>
+      <c r="T25" s="46">
+        <v>0</v>
+      </c>
+      <c r="U25" s="46">
+        <v>0</v>
+      </c>
+      <c r="V25" s="46">
+        <v>0</v>
+      </c>
+      <c r="W25" s="46">
+        <v>0</v>
+      </c>
+      <c r="X25" s="46">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="46">
+        <v>0</v>
+      </c>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8"/>
       <c r="AB25" s="8"/>
@@ -2281,36 +3262,76 @@
       <c r="A26" s="28">
         <v>25</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="32">
         <v>1</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="24"/>
-      <c r="V26" s="24"/>
-      <c r="W26" s="24"/>
-      <c r="X26" s="24"/>
-      <c r="Y26" s="24"/>
+      <c r="F26" s="46">
+        <v>0</v>
+      </c>
+      <c r="G26" s="45">
+        <v>0</v>
+      </c>
+      <c r="H26" s="45">
+        <v>0</v>
+      </c>
+      <c r="I26" s="46">
+        <v>0</v>
+      </c>
+      <c r="J26" s="46">
+        <v>0</v>
+      </c>
+      <c r="K26" s="46">
+        <v>0</v>
+      </c>
+      <c r="L26" s="46">
+        <v>0</v>
+      </c>
+      <c r="M26" s="46">
+        <v>0</v>
+      </c>
+      <c r="N26" s="46">
+        <v>0</v>
+      </c>
+      <c r="O26" s="46">
+        <v>0</v>
+      </c>
+      <c r="P26" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="46">
+        <v>0</v>
+      </c>
+      <c r="R26" s="46">
+        <v>0</v>
+      </c>
+      <c r="S26" s="46">
+        <v>0</v>
+      </c>
+      <c r="T26" s="46">
+        <v>0</v>
+      </c>
+      <c r="U26" s="46">
+        <v>0</v>
+      </c>
+      <c r="V26" s="46">
+        <v>0</v>
+      </c>
+      <c r="W26" s="46">
+        <v>0</v>
+      </c>
+      <c r="X26" s="46">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="46">
+        <v>0</v>
+      </c>
       <c r="Z26" s="8"/>
       <c r="AA26" s="8"/>
       <c r="AB26" s="8"/>
@@ -2322,36 +3343,76 @@
       <c r="A27" s="28">
         <v>26</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="13" t="s">
         <v>25</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="32">
         <v>1</v>
       </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="24"/>
-      <c r="S27" s="24"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="24"/>
-      <c r="V27" s="24"/>
-      <c r="W27" s="24"/>
-      <c r="X27" s="24"/>
-      <c r="Y27" s="24"/>
+      <c r="F27" s="46">
+        <v>0</v>
+      </c>
+      <c r="G27" s="45">
+        <v>0</v>
+      </c>
+      <c r="H27" s="45">
+        <v>0</v>
+      </c>
+      <c r="I27" s="46">
+        <v>0</v>
+      </c>
+      <c r="J27" s="46">
+        <v>0</v>
+      </c>
+      <c r="K27" s="46">
+        <v>0</v>
+      </c>
+      <c r="L27" s="46">
+        <v>0</v>
+      </c>
+      <c r="M27" s="46">
+        <v>0</v>
+      </c>
+      <c r="N27" s="46">
+        <v>0</v>
+      </c>
+      <c r="O27" s="46">
+        <v>0</v>
+      </c>
+      <c r="P27" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="46">
+        <v>0</v>
+      </c>
+      <c r="R27" s="46">
+        <v>0</v>
+      </c>
+      <c r="S27" s="46">
+        <v>0</v>
+      </c>
+      <c r="T27" s="46">
+        <v>0</v>
+      </c>
+      <c r="U27" s="46">
+        <v>0</v>
+      </c>
+      <c r="V27" s="46">
+        <v>0</v>
+      </c>
+      <c r="W27" s="46">
+        <v>0</v>
+      </c>
+      <c r="X27" s="46">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="46">
+        <v>0</v>
+      </c>
       <c r="Z27" s="8"/>
       <c r="AA27" s="8"/>
       <c r="AB27" s="8"/>
@@ -2363,36 +3424,76 @@
       <c r="A28" s="28">
         <v>27</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="32">
         <v>1</v>
       </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="24"/>
-      <c r="S28" s="24"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="24"/>
-      <c r="V28" s="24"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="24"/>
+      <c r="F28" s="46">
+        <v>0</v>
+      </c>
+      <c r="G28" s="45">
+        <v>0</v>
+      </c>
+      <c r="H28" s="45">
+        <v>0</v>
+      </c>
+      <c r="I28" s="46">
+        <v>0</v>
+      </c>
+      <c r="J28" s="46">
+        <v>0</v>
+      </c>
+      <c r="K28" s="46">
+        <v>0</v>
+      </c>
+      <c r="L28" s="46">
+        <v>0</v>
+      </c>
+      <c r="M28" s="46">
+        <v>0</v>
+      </c>
+      <c r="N28" s="46">
+        <v>0</v>
+      </c>
+      <c r="O28" s="46">
+        <v>0</v>
+      </c>
+      <c r="P28" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="46">
+        <v>0</v>
+      </c>
+      <c r="R28" s="46">
+        <v>0</v>
+      </c>
+      <c r="S28" s="46">
+        <v>0</v>
+      </c>
+      <c r="T28" s="46">
+        <v>0</v>
+      </c>
+      <c r="U28" s="46">
+        <v>0</v>
+      </c>
+      <c r="V28" s="46">
+        <v>0</v>
+      </c>
+      <c r="W28" s="46">
+        <v>0</v>
+      </c>
+      <c r="X28" s="46">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="46">
+        <v>0</v>
+      </c>
       <c r="Z28" s="8"/>
       <c r="AA28" s="8"/>
       <c r="AB28" s="8"/>
@@ -2411,29 +3512,69 @@
       <c r="D29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="32">
         <v>1</v>
       </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-      <c r="L29" s="17"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
-      <c r="S29" s="17"/>
-      <c r="T29" s="17"/>
-      <c r="U29" s="17"/>
-      <c r="V29" s="17"/>
-      <c r="W29" s="17"/>
-      <c r="X29" s="17"/>
-      <c r="Y29" s="17"/>
+      <c r="F29" s="46">
+        <v>0</v>
+      </c>
+      <c r="G29" s="45">
+        <v>0</v>
+      </c>
+      <c r="H29" s="45">
+        <v>0</v>
+      </c>
+      <c r="I29" s="46">
+        <v>0</v>
+      </c>
+      <c r="J29" s="46">
+        <v>0</v>
+      </c>
+      <c r="K29" s="46">
+        <v>0</v>
+      </c>
+      <c r="L29" s="46">
+        <v>0</v>
+      </c>
+      <c r="M29" s="46">
+        <v>0</v>
+      </c>
+      <c r="N29" s="46">
+        <v>0</v>
+      </c>
+      <c r="O29" s="46">
+        <v>0</v>
+      </c>
+      <c r="P29" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="46">
+        <v>0</v>
+      </c>
+      <c r="R29" s="46">
+        <v>0</v>
+      </c>
+      <c r="S29" s="46">
+        <v>0</v>
+      </c>
+      <c r="T29" s="46">
+        <v>0</v>
+      </c>
+      <c r="U29" s="46">
+        <v>0</v>
+      </c>
+      <c r="V29" s="46">
+        <v>0</v>
+      </c>
+      <c r="W29" s="46">
+        <v>0</v>
+      </c>
+      <c r="X29" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="46">
+        <v>1</v>
+      </c>
       <c r="Z29" s="9"/>
       <c r="AA29" s="9"/>
       <c r="AB29" s="9"/>
@@ -2452,29 +3593,69 @@
       <c r="D30" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="32">
         <v>1</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
-      <c r="S30" s="17"/>
-      <c r="T30" s="17"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="17"/>
-      <c r="W30" s="17"/>
-      <c r="X30" s="17"/>
-      <c r="Y30" s="17"/>
+      <c r="F30" s="46">
+        <v>0</v>
+      </c>
+      <c r="G30" s="45">
+        <v>0</v>
+      </c>
+      <c r="H30" s="45">
+        <v>0</v>
+      </c>
+      <c r="I30" s="46">
+        <v>0</v>
+      </c>
+      <c r="J30" s="46">
+        <v>0</v>
+      </c>
+      <c r="K30" s="46">
+        <v>0</v>
+      </c>
+      <c r="L30" s="46">
+        <v>0</v>
+      </c>
+      <c r="M30" s="46">
+        <v>0</v>
+      </c>
+      <c r="N30" s="46">
+        <v>0</v>
+      </c>
+      <c r="O30" s="46">
+        <v>0</v>
+      </c>
+      <c r="P30" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="46">
+        <v>0</v>
+      </c>
+      <c r="R30" s="46">
+        <v>0</v>
+      </c>
+      <c r="S30" s="46">
+        <v>0</v>
+      </c>
+      <c r="T30" s="46">
+        <v>0</v>
+      </c>
+      <c r="U30" s="46">
+        <v>0</v>
+      </c>
+      <c r="V30" s="46">
+        <v>0</v>
+      </c>
+      <c r="W30" s="46">
+        <v>0</v>
+      </c>
+      <c r="X30" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="46">
+        <v>1</v>
+      </c>
       <c r="Z30" s="9"/>
       <c r="AA30" s="9"/>
       <c r="AB30" s="9"/>
@@ -2493,29 +3674,69 @@
       <c r="D31" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="32">
         <v>1</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
-      <c r="S31" s="17"/>
-      <c r="T31" s="17"/>
-      <c r="U31" s="17"/>
-      <c r="V31" s="17"/>
-      <c r="W31" s="17"/>
-      <c r="X31" s="17"/>
-      <c r="Y31" s="17"/>
+      <c r="F31" s="46">
+        <v>0</v>
+      </c>
+      <c r="G31" s="45">
+        <v>0</v>
+      </c>
+      <c r="H31" s="45">
+        <v>0</v>
+      </c>
+      <c r="I31" s="46">
+        <v>0</v>
+      </c>
+      <c r="J31" s="46">
+        <v>0</v>
+      </c>
+      <c r="K31" s="46">
+        <v>0</v>
+      </c>
+      <c r="L31" s="46">
+        <v>0</v>
+      </c>
+      <c r="M31" s="46">
+        <v>0</v>
+      </c>
+      <c r="N31" s="46">
+        <v>0</v>
+      </c>
+      <c r="O31" s="46">
+        <v>0</v>
+      </c>
+      <c r="P31" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="46">
+        <v>0</v>
+      </c>
+      <c r="R31" s="46">
+        <v>0</v>
+      </c>
+      <c r="S31" s="46">
+        <v>0</v>
+      </c>
+      <c r="T31" s="46">
+        <v>0</v>
+      </c>
+      <c r="U31" s="46">
+        <v>0</v>
+      </c>
+      <c r="V31" s="46">
+        <v>0</v>
+      </c>
+      <c r="W31" s="46">
+        <v>0</v>
+      </c>
+      <c r="X31" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="46">
+        <v>1</v>
+      </c>
       <c r="Z31" s="9"/>
       <c r="AA31" s="9"/>
       <c r="AB31" s="9"/>
@@ -2534,29 +3755,69 @@
       <c r="D32" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="32">
         <v>1</v>
       </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="17"/>
-      <c r="Y32" s="17"/>
+      <c r="F32" s="46">
+        <v>0</v>
+      </c>
+      <c r="G32" s="45">
+        <v>0</v>
+      </c>
+      <c r="H32" s="45">
+        <v>0</v>
+      </c>
+      <c r="I32" s="46">
+        <v>0</v>
+      </c>
+      <c r="J32" s="46">
+        <v>0</v>
+      </c>
+      <c r="K32" s="46">
+        <v>0</v>
+      </c>
+      <c r="L32" s="46">
+        <v>0</v>
+      </c>
+      <c r="M32" s="46">
+        <v>0</v>
+      </c>
+      <c r="N32" s="46">
+        <v>0</v>
+      </c>
+      <c r="O32" s="46">
+        <v>0</v>
+      </c>
+      <c r="P32" s="46">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="46">
+        <v>0</v>
+      </c>
+      <c r="R32" s="46">
+        <v>0</v>
+      </c>
+      <c r="S32" s="46">
+        <v>0</v>
+      </c>
+      <c r="T32" s="46">
+        <v>0</v>
+      </c>
+      <c r="U32" s="46">
+        <v>0</v>
+      </c>
+      <c r="V32" s="46">
+        <v>0</v>
+      </c>
+      <c r="W32" s="46">
+        <v>0</v>
+      </c>
+      <c r="X32" s="46">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="46">
+        <v>1</v>
+      </c>
       <c r="Z32" s="9"/>
       <c r="AA32" s="9"/>
       <c r="AB32" s="9"/>
@@ -2564,91 +3825,96 @@
       <c r="AD32" s="9"/>
       <c r="AE32" s="8"/>
     </row>
-    <row r="33" spans="1:31" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="3">
+        <f>SUM(E2:E32)</f>
+        <v>76</v>
+      </c>
       <c r="F33" s="2">
         <f t="shared" ref="F33:Y33" si="0">SUM(F2:F32)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="T33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y33" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Z33" s="8"/>
       <c r="AA33" s="8"/>
@@ -2656,12 +3922,6 @@
       <c r="AC33" s="8"/>
       <c r="AD33" s="8"/>
       <c r="AE33" s="8"/>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="D38">
-        <f>SUM(E2:E32)</f>
-        <v>76</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2797,7 +4057,7 @@
       <c r="A2" s="30">
         <v>1</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="14" t="s">
         <v>6</v>
       </c>
@@ -2835,7 +4095,7 @@
       <c r="A3" s="30">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
+      <c r="B3" s="33"/>
       <c r="C3" s="14" t="s">
         <v>18</v>
       </c>
@@ -2871,7 +4131,7 @@
       <c r="A4" s="30">
         <v>3</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -2909,7 +4169,7 @@
       <c r="A5" s="30">
         <v>4</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="33"/>
       <c r="C5" s="14" t="s">
         <v>30</v>
       </c>
@@ -2945,7 +4205,7 @@
       <c r="A6" s="30">
         <v>5</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="14" t="s">
         <v>31</v>
       </c>
@@ -2981,7 +4241,7 @@
       <c r="A7" s="30">
         <v>6</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="14" t="s">
         <v>32</v>
       </c>
@@ -3017,7 +4277,7 @@
       <c r="A8" s="30">
         <v>7</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -3053,7 +4313,7 @@
       <c r="A9" s="30">
         <v>8</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="14" t="s">
         <v>38</v>
       </c>
@@ -3087,7 +4347,7 @@
       <c r="A10" s="30">
         <v>9</v>
       </c>
-      <c r="B10" s="35"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="14" t="s">
         <v>40</v>
       </c>
@@ -3121,7 +4381,7 @@
       <c r="A11" s="30">
         <v>10</v>
       </c>
-      <c r="B11" s="35"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="14" t="s">
         <v>39</v>
       </c>
@@ -3155,7 +4415,7 @@
       <c r="A12" s="30">
         <v>11</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="37" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -3191,7 +4451,7 @@
       <c r="A13" s="30">
         <v>12</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="14" t="s">
         <v>41</v>
       </c>
@@ -3225,7 +4485,7 @@
       <c r="A14" s="30">
         <v>13</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="20" t="s">
         <v>42</v>
       </c>
@@ -3259,7 +4519,7 @@
       <c r="A15" s="30">
         <v>14</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="34" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="21" t="s">
@@ -3295,7 +4555,7 @@
       <c r="A16" s="30">
         <v>15</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="14" t="s">
         <v>44</v>
       </c>
@@ -3329,7 +4589,7 @@
       <c r="A17" s="30">
         <v>16</v>
       </c>
-      <c r="B17" s="32"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
@@ -3363,7 +4623,7 @@
       <c r="A18" s="30">
         <v>17</v>
       </c>
-      <c r="B18" s="34"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
@@ -3397,7 +4657,7 @@
       <c r="A19" s="30">
         <v>18</v>
       </c>
-      <c r="B19" s="33" t="s">
+      <c r="B19" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -3433,7 +4693,7 @@
       <c r="A20" s="30">
         <v>19</v>
       </c>
-      <c r="B20" s="32"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="14" t="s">
         <v>21</v>
       </c>
@@ -3467,7 +4727,7 @@
       <c r="A21" s="30">
         <v>20</v>
       </c>
-      <c r="B21" s="34"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="14" t="s">
         <v>21</v>
       </c>
@@ -3501,7 +4761,7 @@
       <c r="A22" s="30">
         <v>21</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="13" t="s">
         <v>8</v>
       </c>
@@ -3535,7 +4795,7 @@
       <c r="A23" s="30">
         <v>22</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="36"/>
       <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
@@ -3569,7 +4829,7 @@
       <c r="A24" s="30">
         <v>23</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="36"/>
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
@@ -3603,7 +4863,7 @@
       <c r="A25" s="30">
         <v>24</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="36"/>
       <c r="C25" s="4" t="s">
         <v>23</v>
       </c>
@@ -3637,7 +4897,7 @@
       <c r="A26" s="30">
         <v>25</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="4" t="s">
         <v>24</v>
       </c>
@@ -3671,7 +4931,7 @@
       <c r="A27" s="30">
         <v>26</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="13" t="s">
         <v>25</v>
       </c>
@@ -3705,7 +4965,7 @@
       <c r="A28" s="30">
         <v>27</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="13" t="s">
         <v>26</v>
       </c>
@@ -3874,8 +5134,8 @@
     <row r="33" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="39"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
         <v>14</v>

</xml_diff>